<commit_message>
1. Se realiza cambios en modelo de flujo de procesos en drawio. 2. Se agrega nuevos comentarios en decisiones de las decisiones tomadas    y mayores  desafios encontrados. 3. Se realizan cambios en lectura excel donde se guarda la tabla    Vencimientos de la base de datos. Se hace relación con lo modelado  y se hacen    modificaciones adicionales en su propia rama. 4. Se realiza test donde se obtiene los jquery se comienza con la    grafica 1.
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Fechas_Indicadores.xlsx
+++ b/app/dataextraction/Recibos/Fechas_Indicadores.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E722C036-DE8A-484E-9AAB-66685F1D53D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8324A3-8D95-40CD-962B-31E246CA413F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13908" yWindow="180" windowWidth="8184" windowHeight="12180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Clientes  BORRADOR" sheetId="1" r:id="rId1"/>
+    <sheet name="Clientes " sheetId="1" r:id="rId1"/>
     <sheet name="Tablas indicadores y graficos" sheetId="3" r:id="rId2"/>
     <sheet name="Clientes  Trabajar" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Tablas consulta" sheetId="7" r:id="rId4"/>
+    <sheet name="chart" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Clientes  BORRADOR'!$A$1:$P$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Clientes '!$A$1:$I$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Clientes  Trabajar'!$A$159:$P$173</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="163">
   <si>
     <t>pais</t>
   </si>
@@ -510,6 +511,27 @@
   <si>
     <t>elegir la de arriba porque se puede leer la q esta elegida no</t>
   </si>
+  <si>
+    <t>lista_procesadopdf=</t>
+  </si>
+  <si>
+    <t>clv</t>
+  </si>
+  <si>
+    <t>lista_extraccExcel=</t>
+  </si>
+  <si>
+    <t>mes</t>
+  </si>
+  <si>
+    <t>proceso</t>
+  </si>
+  <si>
+    <t>años</t>
+  </si>
+  <si>
+    <t>grafico1</t>
+  </si>
 </sst>
 </file>
 
@@ -519,7 +541,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,6 +651,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Cascadia Code PL"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF7030A0"/>
+      <name val="Cascadia Code PL"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -715,7 +750,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -817,6 +852,17 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3438,7 +3484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C9D996B-E4E2-46FE-854A-DE3FEC62DD62}" type="CELLRANGE">
+                    <a:fld id="{58C09E27-338E-4EA3-BC4D-35800720EB5A}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3447,7 +3493,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{1F75BC40-DB81-4292-8662-B277B2C18844}" type="PERCENTAGE">
+                    <a:fld id="{13899A89-94E2-4F6F-9BAB-E8F0118D8196}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3480,7 +3526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA2BA243-0FE6-41F2-882C-797AED87169D}" type="CELLRANGE">
+                    <a:fld id="{5885551E-F647-4619-88C8-8A234BC3A1AF}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3489,7 +3535,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{45975594-61B1-4850-9C68-826A73AE8255}" type="PERCENTAGE">
+                    <a:fld id="{BD2BD9D5-FAFD-4923-AC81-8233F5AF65E1}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3522,7 +3568,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB8E0EE1-A84E-4B51-A1C3-2D70E85B7AC2}" type="CELLRANGE">
+                    <a:fld id="{ED835CEE-9BB3-4A27-B547-5826209068BD}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3531,7 +3577,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{26BFF3DD-DBA7-4EB4-A192-52D5DE7263CE}" type="PERCENTAGE">
+                    <a:fld id="{B8968502-56BA-49F8-9F4E-38BF16AAD829}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3896,7 +3942,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1C2B1D9-D29F-421C-98FB-1E109538B364}" type="CELLRANGE">
+                    <a:fld id="{74435343-AC85-43AC-B9E1-243E6696F717}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3905,7 +3951,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{D9BE2256-6D64-44C6-BB9D-7096E841A963}" type="PERCENTAGE">
+                    <a:fld id="{001D7DB2-E0E8-46EB-8DF4-92F40E99FCEF}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3938,7 +3984,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCE0769B-A957-41CD-AF93-736A09A3B132}" type="CELLRANGE">
+                    <a:fld id="{09D2820D-A40E-4E14-871D-7CE18CD9E621}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3947,7 +3993,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{7D44F665-F352-4D94-891E-B3CE66DA82D7}" type="PERCENTAGE">
+                    <a:fld id="{81814BE4-5701-4762-BDD5-734D30045414}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3980,7 +4026,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B57B0C68-9D31-4570-90F3-D9B6884ED4E8}" type="CELLRANGE">
+                    <a:fld id="{881AC11D-FF9A-49EE-AB29-25F8E8334F89}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3989,7 +4035,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{7D363CC7-D2DA-4F42-B063-A7198096D2E9}" type="PERCENTAGE">
+                    <a:fld id="{C8754553-48AA-4975-9B64-B5BE67CFBA6C}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -7871,6 +7917,99 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>396128</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>565184</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8314A0D0-99C2-59D6-8E20-B03940611020}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8961008" y="0"/>
+          <a:ext cx="2607456" cy="1889760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>102810</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>517511</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>117650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68C7ED12-12DC-33BD-6127-B8934730F82E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9886890" y="2034540"/>
+          <a:ext cx="3462701" cy="2456990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -8095,7 +8234,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="jazmin" refreshedDate="44816.71880023148" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="44" xr:uid="{2B73D9EC-2D7D-4723-81E4-5D0CDBA495BA}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:Q45" sheet="Clientes  BORRADOR"/>
+    <worksheetSource ref="A1:I45" sheet="Clientes "/>
   </cacheSource>
   <cacheFields count="18">
     <cacheField name="pais" numFmtId="0">
@@ -12602,10 +12741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12616,38 +12755,41 @@
     <col min="4" max="5" width="7.5546875" style="6" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="6"/>
+    <col min="9" max="9" width="15.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="6"/>
+    <col min="11" max="11" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="63" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="63" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="8" t="s">
@@ -12699,7 +12841,7 @@
         <v>44628</v>
       </c>
       <c r="H2" s="16">
-        <f t="shared" ref="H2:H23" si="1">+G2-1</f>
+        <f t="shared" ref="H2:H34" si="1">+G2-1</f>
         <v>44627</v>
       </c>
       <c r="I2" s="14" t="s">
@@ -12740,10 +12882,10 @@
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="3">
@@ -12757,13 +12899,13 @@
         <f t="shared" si="1"/>
         <v>44631</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="6">
         <v>2022</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="6">
         <v>731</v>
       </c>
       <c r="L3" s="12" t="s">
@@ -12781,11 +12923,11 @@
       <c r="P3" s="23">
         <v>44816</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -12809,7 +12951,7 @@
         <v>44636</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H6" si="2">+G4-1</f>
+        <f t="shared" si="1"/>
         <v>44635</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -12822,7 +12964,6 @@
         <v>300</v>
       </c>
       <c r="L4" s="12">
-        <f>+L10</f>
         <v>3004648676658</v>
       </c>
       <c r="M4" s="10">
@@ -12841,7 +12982,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -12865,7 +13006,7 @@
         <v>44629</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44628</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -12878,7 +13019,6 @@
         <v>300</v>
       </c>
       <c r="L5" s="12">
-        <f>+L4+1</f>
         <v>3004648676659</v>
       </c>
       <c r="M5" s="10">
@@ -12897,7 +13037,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -12921,7 +13061,7 @@
         <v>44632</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44631</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -12934,7 +13074,6 @@
         <v>300</v>
       </c>
       <c r="L6" s="12">
-        <f>+L5+1</f>
         <v>3004648676660</v>
       </c>
       <c r="M6" s="10">
@@ -12961,10 +13100,10 @@
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="3">
@@ -12978,7 +13117,7 @@
         <f t="shared" si="1"/>
         <v>44625</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="6">
@@ -13016,10 +13155,10 @@
       <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="3">
@@ -13033,7 +13172,7 @@
         <f t="shared" si="1"/>
         <v>44633</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="6">
@@ -13071,10 +13210,10 @@
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="3">
@@ -13088,7 +13227,7 @@
         <f t="shared" si="1"/>
         <v>44632</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J9" s="6">
@@ -13236,24 +13375,24 @@
       <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>2</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="3">
         <v>44637</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" ref="G12:G18" si="3">+F12-3</f>
+        <f t="shared" ref="G12:G18" si="2">+F12-3</f>
         <v>44634</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="1"/>
         <v>44633</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J12" s="6">
@@ -13281,7 +13420,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -13301,7 +13440,7 @@
         <v>44639</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44636</v>
       </c>
       <c r="H13" s="3">
@@ -13318,7 +13457,6 @@
         <v>300</v>
       </c>
       <c r="L13" s="12">
-        <f>+L10</f>
         <v>3004648676658</v>
       </c>
       <c r="M13" s="10">
@@ -13337,7 +13475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -13357,7 +13495,7 @@
         <v>44632</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44629</v>
       </c>
       <c r="H14" s="3">
@@ -13374,7 +13512,6 @@
         <v>300</v>
       </c>
       <c r="L14" s="12">
-        <f>+L13+1</f>
         <v>3004648676659</v>
       </c>
       <c r="M14" s="10">
@@ -13393,7 +13530,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -13413,7 +13550,7 @@
         <v>44635</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44632</v>
       </c>
       <c r="H15" s="3">
@@ -13430,7 +13567,6 @@
         <v>300</v>
       </c>
       <c r="L15" s="12">
-        <f>+L14+1</f>
         <v>3004648676660</v>
       </c>
       <c r="M15" s="10">
@@ -13447,7 +13583,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -13467,11 +13603,11 @@
         <v>44603</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44600</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" ref="H16:H21" si="4">+G16-1</f>
+        <f t="shared" si="1"/>
         <v>44599</v>
       </c>
       <c r="I16" s="6" t="s">
@@ -13483,9 +13619,8 @@
       <c r="K16" s="6">
         <v>731</v>
       </c>
-      <c r="L16" s="12" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
+      <c r="L16" s="12">
+        <v>3004648676661</v>
       </c>
       <c r="M16" s="10">
         <v>3313414.59</v>
@@ -13504,7 +13639,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
@@ -13524,11 +13659,11 @@
         <v>44607</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44604</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>44603</v>
       </c>
       <c r="I17" s="6" t="s">
@@ -13540,9 +13675,8 @@
       <c r="K17" s="6">
         <v>731</v>
       </c>
-      <c r="L17" s="12" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
+      <c r="L17" s="12">
+        <v>3004648676662</v>
       </c>
       <c r="M17" s="10">
         <v>0</v>
@@ -13554,14 +13688,14 @@
         <v>12</v>
       </c>
       <c r="P17" s="23">
-        <f t="shared" ref="P17:P19" si="5">+F17-1</f>
+        <f t="shared" ref="P17:P19" si="3">+F17-1</f>
         <v>44606</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
@@ -13581,11 +13715,11 @@
         <v>44601</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44598</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>44597</v>
       </c>
       <c r="I18" s="6" t="s">
@@ -13597,9 +13731,8 @@
       <c r="K18" s="6">
         <v>731</v>
       </c>
-      <c r="L18" s="12" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
+      <c r="L18" s="12">
+        <v>3004648676663</v>
       </c>
       <c r="M18" s="10">
         <v>5635000</v>
@@ -13611,14 +13744,14 @@
         <v>12</v>
       </c>
       <c r="P18" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>44600</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -13642,7 +13775,7 @@
         <v>44606</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>44605</v>
       </c>
       <c r="I19" s="6" t="s">
@@ -13654,9 +13787,8 @@
       <c r="K19" s="6">
         <v>731</v>
       </c>
-      <c r="L19" s="12" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
+      <c r="L19" s="12">
+        <v>3004648676664</v>
       </c>
       <c r="M19" s="10">
         <v>0</v>
@@ -13668,14 +13800,14 @@
         <v>12</v>
       </c>
       <c r="P19" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>44606</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
@@ -13699,7 +13831,7 @@
         <v>44600</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>44599</v>
       </c>
       <c r="I20" s="6" t="s">
@@ -13711,9 +13843,8 @@
       <c r="K20" s="6">
         <v>731</v>
       </c>
-      <c r="L20" s="12" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
+      <c r="L20" s="12">
+        <v>3004648676665</v>
       </c>
       <c r="M20" s="10">
         <v>3313414.59</v>
@@ -13732,7 +13863,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
@@ -13756,7 +13887,7 @@
         <v>44604</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>44603</v>
       </c>
       <c r="I21" s="6" t="s">
@@ -13768,9 +13899,8 @@
       <c r="K21" s="6">
         <v>731</v>
       </c>
-      <c r="L21" s="12" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
+      <c r="L21" s="12">
+        <v>3004648676666</v>
       </c>
       <c r="M21" s="10">
         <v>0</v>
@@ -13782,14 +13912,14 @@
         <v>12</v>
       </c>
       <c r="P21" s="23">
-        <f t="shared" ref="P21" si="6">+F21-1</f>
+        <f t="shared" ref="P21:P23" si="4">+F21-1</f>
         <v>44606</v>
       </c>
       <c r="Q21" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
@@ -13825,9 +13955,8 @@
       <c r="K22" s="6">
         <v>731</v>
       </c>
-      <c r="L22" s="12" t="e">
-        <f>+#REF!</f>
-        <v>#REF!</v>
+      <c r="L22" s="12">
+        <v>3004648676667</v>
       </c>
       <c r="M22" s="10">
         <v>5635000</v>
@@ -13839,14 +13968,14 @@
         <v>12</v>
       </c>
       <c r="P22" s="23">
-        <f t="shared" ref="P22:P23" si="7">+F22-1</f>
+        <f t="shared" si="4"/>
         <v>44600</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
@@ -13882,9 +14011,8 @@
       <c r="K23" s="6">
         <v>731</v>
       </c>
-      <c r="L23" s="12" t="str">
-        <f>+L1</f>
-        <v xml:space="preserve"> n_verificacion</v>
+      <c r="L23" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="M23" s="10">
         <v>0</v>
@@ -13896,14 +14024,14 @@
         <v>12</v>
       </c>
       <c r="P23" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>44606</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>9</v>
       </c>
@@ -13927,7 +14055,7 @@
         <v>44600</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" ref="H24:H34" si="8">+G24-1</f>
+        <f t="shared" si="1"/>
         <v>44599</v>
       </c>
       <c r="I24" s="6" t="s">
@@ -13939,9 +14067,8 @@
       <c r="K24" s="6">
         <v>731</v>
       </c>
-      <c r="L24" s="12" t="str">
-        <f>+L2</f>
-        <v>146752/201103</v>
+      <c r="L24" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="M24" s="10">
         <v>3313414.59</v>
@@ -13960,7 +14087,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
@@ -13984,7 +14111,7 @@
         <v>44604</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44603</v>
       </c>
       <c r="I25" s="6" t="s">
@@ -13996,9 +14123,8 @@
       <c r="K25" s="6">
         <v>731</v>
       </c>
-      <c r="L25" s="12" t="str">
-        <f>+L3</f>
-        <v>146753/201104</v>
+      <c r="L25" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="M25" s="10">
         <v>0</v>
@@ -14010,14 +14136,14 @@
         <v>12</v>
       </c>
       <c r="P25" s="23">
-        <f t="shared" ref="P25:P34" si="9">+F25-1</f>
+        <f t="shared" ref="P25:P34" si="5">+F25-1</f>
         <v>44606</v>
       </c>
       <c r="Q25" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -14041,7 +14167,7 @@
         <v>44598</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44597</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -14053,9 +14179,8 @@
       <c r="K26" s="6">
         <v>731</v>
       </c>
-      <c r="L26" s="12" t="str">
-        <f t="shared" ref="L26:L34" si="10">+L7</f>
-        <v>146754/201105</v>
+      <c r="L26" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="M26" s="10">
         <v>5635000</v>
@@ -14067,14 +14192,14 @@
         <v>12</v>
       </c>
       <c r="P26" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44600</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
@@ -14098,7 +14223,7 @@
         <v>44606</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44605</v>
       </c>
       <c r="I27" s="6" t="s">
@@ -14110,9 +14235,8 @@
       <c r="K27" s="6">
         <v>731</v>
       </c>
-      <c r="L27" s="12" t="str">
-        <f t="shared" si="10"/>
-        <v>146755/201106</v>
+      <c r="L27" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="M27" s="10">
         <v>0</v>
@@ -14124,14 +14248,14 @@
         <v>12</v>
       </c>
       <c r="P27" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44606</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
@@ -14155,7 +14279,7 @@
         <v>44605</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44604</v>
       </c>
       <c r="I28" s="6" t="s">
@@ -14167,9 +14291,8 @@
       <c r="K28" s="6">
         <v>731</v>
       </c>
-      <c r="L28" s="12" t="str">
-        <f t="shared" si="10"/>
-        <v>146756/201107</v>
+      <c r="L28" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="M28" s="10">
         <v>5313414.59</v>
@@ -14181,14 +14304,14 @@
         <v>12</v>
       </c>
       <c r="P28" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44607</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
@@ -14212,7 +14335,7 @@
         <v>44605</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44604</v>
       </c>
       <c r="I29" s="6" t="s">
@@ -14225,7 +14348,6 @@
         <v>300</v>
       </c>
       <c r="L29" s="12">
-        <f t="shared" si="10"/>
         <v>3004648676658</v>
       </c>
       <c r="M29" s="10">
@@ -14238,14 +14360,14 @@
         <v>12</v>
       </c>
       <c r="P29" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44606</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
@@ -14269,7 +14391,7 @@
         <v>44609</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44608</v>
       </c>
       <c r="I30" s="6" t="s">
@@ -14282,7 +14404,6 @@
         <v>1</v>
       </c>
       <c r="L30" s="12">
-        <f t="shared" si="10"/>
         <v>220060080649</v>
       </c>
       <c r="M30" s="10">
@@ -14295,14 +14416,14 @@
         <v>30</v>
       </c>
       <c r="P30" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44610</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
@@ -14322,11 +14443,11 @@
         <v>44609</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" ref="G31:G37" si="11">+F31-3</f>
+        <f t="shared" ref="G31:G37" si="6">+F31-3</f>
         <v>44606</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44605</v>
       </c>
       <c r="I31" s="6" t="s">
@@ -14338,9 +14459,8 @@
       <c r="K31" s="6">
         <v>731</v>
       </c>
-      <c r="L31" s="12" t="str">
-        <f t="shared" si="10"/>
-        <v>146759/201110</v>
+      <c r="L31" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="M31" s="10">
         <v>4313414.59</v>
@@ -14352,14 +14472,14 @@
         <v>12</v>
       </c>
       <c r="P31" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44608</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>25</v>
       </c>
@@ -14379,11 +14499,11 @@
         <v>44611</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>44608</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44607</v>
       </c>
       <c r="I32" s="6" t="s">
@@ -14396,7 +14516,6 @@
         <v>300</v>
       </c>
       <c r="L32" s="12">
-        <f t="shared" si="10"/>
         <v>3004648676658</v>
       </c>
       <c r="M32" s="10">
@@ -14409,14 +14528,14 @@
         <v>12</v>
       </c>
       <c r="P32" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44610</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>25</v>
       </c>
@@ -14436,11 +14555,11 @@
         <v>44604</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>44601</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44600</v>
       </c>
       <c r="I33" s="6" t="s">
@@ -14453,7 +14572,6 @@
         <v>300</v>
       </c>
       <c r="L33" s="12">
-        <f t="shared" si="10"/>
         <v>3004648676659</v>
       </c>
       <c r="M33" s="10">
@@ -14466,14 +14584,14 @@
         <v>12</v>
       </c>
       <c r="P33" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44603</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>25</v>
       </c>
@@ -14493,11 +14611,11 @@
         <v>44607</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>44604</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>44603</v>
       </c>
       <c r="I34" s="6" t="s">
@@ -14510,7 +14628,6 @@
         <v>300</v>
       </c>
       <c r="L34" s="12">
-        <f t="shared" si="10"/>
         <v>3004648676660</v>
       </c>
       <c r="M34" s="10">
@@ -14521,14 +14638,14 @@
         <v>12</v>
       </c>
       <c r="P34" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>44606</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>9</v>
       </c>
@@ -14548,7 +14665,7 @@
         <v>44572</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>44569</v>
       </c>
       <c r="H35" s="3">
@@ -14563,9 +14680,8 @@
       <c r="K35" s="6">
         <v>731</v>
       </c>
-      <c r="L35" s="12" t="str">
-        <f>+L24</f>
-        <v>146752/201103</v>
+      <c r="L35" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="M35" s="10">
         <v>3313414.59</v>
@@ -14584,7 +14700,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>9</v>
       </c>
@@ -14604,7 +14720,7 @@
         <v>44576</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>44573</v>
       </c>
       <c r="H36" s="3">
@@ -14619,9 +14735,8 @@
       <c r="K36" s="6">
         <v>731</v>
       </c>
-      <c r="L36" s="12" t="str">
-        <f t="shared" ref="L36:L45" si="12">+L25</f>
-        <v>146753/201104</v>
+      <c r="L36" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="M36" s="10">
         <v>0</v>
@@ -14633,14 +14748,14 @@
         <v>12</v>
       </c>
       <c r="P36" s="23">
-        <f t="shared" ref="P36:P45" si="13">+F36-1</f>
+        <f t="shared" ref="P36:P45" si="7">+F36-1</f>
         <v>44575</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>9</v>
       </c>
@@ -14660,7 +14775,7 @@
         <v>44570</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>44567</v>
       </c>
       <c r="H37" s="3">
@@ -14675,9 +14790,8 @@
       <c r="K37" s="6">
         <v>731</v>
       </c>
-      <c r="L37" s="12" t="str">
-        <f t="shared" si="12"/>
-        <v>146754/201105</v>
+      <c r="L37" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="M37" s="10">
         <v>5635000</v>
@@ -14689,14 +14803,14 @@
         <v>12</v>
       </c>
       <c r="P37" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44569</v>
       </c>
       <c r="Q37" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -14731,9 +14845,8 @@
       <c r="K38" s="6">
         <v>731</v>
       </c>
-      <c r="L38" s="12" t="str">
-        <f t="shared" si="12"/>
-        <v>146755/201106</v>
+      <c r="L38" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="M38" s="10">
         <v>0</v>
@@ -14745,14 +14858,14 @@
         <v>12</v>
       </c>
       <c r="P38" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44575</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>9</v>
       </c>
@@ -14787,9 +14900,8 @@
       <c r="K39" s="6">
         <v>731</v>
       </c>
-      <c r="L39" s="12" t="str">
-        <f t="shared" si="12"/>
-        <v>146756/201107</v>
+      <c r="L39" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="M39" s="10">
         <v>5313414.59</v>
@@ -14801,14 +14913,14 @@
         <v>12</v>
       </c>
       <c r="P39" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44576</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>25</v>
       </c>
@@ -14844,7 +14956,6 @@
         <v>300</v>
       </c>
       <c r="L40" s="12">
-        <f t="shared" si="12"/>
         <v>3004648676658</v>
       </c>
       <c r="M40" s="10">
@@ -14857,14 +14968,14 @@
         <v>12</v>
       </c>
       <c r="P40" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44575</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
@@ -14900,7 +15011,6 @@
         <v>1</v>
       </c>
       <c r="L41" s="12">
-        <f t="shared" si="12"/>
         <v>220060080649</v>
       </c>
       <c r="M41" s="10">
@@ -14913,14 +15023,14 @@
         <v>30</v>
       </c>
       <c r="P41" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44579</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
@@ -14955,9 +15065,8 @@
       <c r="K42" s="6">
         <v>731</v>
       </c>
-      <c r="L42" s="12" t="str">
-        <f t="shared" si="12"/>
-        <v>146759/201110</v>
+      <c r="L42" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="M42" s="10">
         <v>4313414.59</v>
@@ -14969,14 +15078,14 @@
         <v>12</v>
       </c>
       <c r="P42" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44577</v>
       </c>
       <c r="Q42" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>25</v>
       </c>
@@ -15012,7 +15121,6 @@
         <v>300</v>
       </c>
       <c r="L43" s="12">
-        <f t="shared" si="12"/>
         <v>3004648676658</v>
       </c>
       <c r="M43" s="10">
@@ -15025,14 +15133,14 @@
         <v>12</v>
       </c>
       <c r="P43" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44579</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>25</v>
       </c>
@@ -15068,7 +15176,6 @@
         <v>300</v>
       </c>
       <c r="L44" s="12">
-        <f t="shared" si="12"/>
         <v>3004648676659</v>
       </c>
       <c r="M44" s="10">
@@ -15081,14 +15188,14 @@
         <v>12</v>
       </c>
       <c r="P44" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44572</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>25</v>
       </c>
@@ -15124,7 +15231,6 @@
         <v>300</v>
       </c>
       <c r="L45" s="12">
-        <f t="shared" si="12"/>
         <v>3004648676660</v>
       </c>
       <c r="M45" s="10">
@@ -15135,38 +15241,12 @@
         <v>12</v>
       </c>
       <c r="P45" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>44575</v>
       </c>
       <c r="Q45" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="P46" s="23"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="P47" s="23"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="P48" s="23"/>
-    </row>
-    <row r="49" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H49" s="23"/>
-      <c r="P49" s="23"/>
-    </row>
-    <row r="50" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H50" s="23"/>
-      <c r="P50" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15177,8 +15257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1930402-D799-4BFF-9E29-635AB75B75C8}">
   <dimension ref="A2:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N71" sqref="N71"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15854,8 +15934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6A182A-4FB5-4415-8AA7-37C1E232FE20}">
   <dimension ref="A1:AF203"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A173" sqref="A173"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18368,8 +18448,10 @@
       <c r="D59"/>
       <c r="E59"/>
     </row>
-    <row r="60" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C60"/>
+    <row r="60" spans="3:16" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="C60" s="67" t="s">
+        <v>162</v>
+      </c>
       <c r="D60"/>
       <c r="E60"/>
     </row>
@@ -19183,7 +19265,7 @@
       <c r="I112" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J112" s="5" t="s">
+      <c r="J112" s="8" t="s">
         <v>126</v>
       </c>
       <c r="L112" s="5"/>
@@ -19936,7 +20018,7 @@
       <c r="I131" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J131" s="5" t="s">
+      <c r="J131" s="8" t="s">
         <v>127</v>
       </c>
       <c r="N131" s="6" t="s">
@@ -21427,10 +21509,505 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E55A6F8-391D-47CE-A511-E488A5F39536}">
+  <dimension ref="A1:O18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="65"/>
+      <c r="B2" s="66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="16">
+        <v>44631</v>
+      </c>
+      <c r="G4" s="16">
+        <f t="shared" ref="G4:G8" si="0">+F4-3</f>
+        <v>44628</v>
+      </c>
+      <c r="H4" s="16">
+        <f t="shared" ref="H4:H8" si="1">+G4-1</f>
+        <v>44627</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44635</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>44632</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="1"/>
+        <v>44631</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="30">
+        <v>9013543200</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44639</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>44636</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>44635</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="30">
+        <v>9013161451</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44632</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>44629</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="1"/>
+        <v>44628</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="30">
+        <v>9014115458</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3">
+        <v>44635</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>44632</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="1"/>
+        <v>44631</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A12" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="14">
+        <v>2022</v>
+      </c>
+      <c r="D13" s="14">
+        <v>731</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="17">
+        <v>3313414.59</v>
+      </c>
+      <c r="G13" s="17">
+        <v>0</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="3">
+        <v>44816</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2022</v>
+      </c>
+      <c r="D14" s="6">
+        <v>731</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>200000</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="3">
+        <v>44816</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="30">
+        <v>9013543200</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2022</v>
+      </c>
+      <c r="D15" s="6">
+        <v>300</v>
+      </c>
+      <c r="E15" s="12">
+        <v>3004648676658</v>
+      </c>
+      <c r="F15" s="10">
+        <v>256200000</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="3">
+        <v>44816</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="30">
+        <v>9013161451</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2022</v>
+      </c>
+      <c r="D16" s="6">
+        <v>300</v>
+      </c>
+      <c r="E16" s="12">
+        <v>3004648676659</v>
+      </c>
+      <c r="F16" s="10">
+        <v>102124000</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="3">
+        <v>44816</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="30">
+        <v>9014115458</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2022</v>
+      </c>
+      <c r="D17" s="6">
+        <v>300</v>
+      </c>
+      <c r="E17" s="12">
+        <v>3004648676660</v>
+      </c>
+      <c r="F17" s="10">
+        <v>4520000</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="3">
+        <v>44816</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2022</v>
+      </c>
+      <c r="D18" s="6">
+        <v>731</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="10">
+        <v>5635000</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="3">
+        <v>44816</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9649D8A5-2E03-4C44-ACB2-E1D98A876909}">
   <dimension ref="B5:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se agrega lógica de visualizaciones según estructura de chart, se recorre los datos de la base de datos y el excel que se procesa y se unifica los datos para traer visualizaciones
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Fechas_Indicadores.xlsx
+++ b/app/dataextraction/Recibos/Fechas_Indicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8324A3-8D95-40CD-962B-31E246CA413F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266935E7-4832-4E41-A845-3CB0CC746813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes " sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="chart" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Clientes '!$A$1:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Clientes '!$A$1:$Q$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Clientes  Trabajar'!$A$159:$P$173</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="166">
   <si>
     <t>pais</t>
   </si>
@@ -532,6 +532,15 @@
   <si>
     <t>grafico1</t>
   </si>
+  <si>
+    <t>grafico 2</t>
+  </si>
+  <si>
+    <t>se debe relacionar periodo fiscal</t>
+  </si>
+  <si>
+    <t>datos_grafico3</t>
+  </si>
 </sst>
 </file>
 
@@ -992,7 +1001,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.2666972149738006E-2"/>
+          <c:y val="2.2020410115340797E-2"/>
+          <c:w val="0.90290972625452104"/>
+          <c:h val="0.77118345774893982"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -3484,7 +3503,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58C09E27-338E-4EA3-BC4D-35800720EB5A}" type="CELLRANGE">
+                    <a:fld id="{37B6BF7C-A9E0-4BF8-9CDD-7059A03AA5CA}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3493,7 +3512,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{13899A89-94E2-4F6F-9BAB-E8F0118D8196}" type="PERCENTAGE">
+                    <a:fld id="{15891FB5-7C87-46C1-A75C-D6327D607D15}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3526,7 +3545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5885551E-F647-4619-88C8-8A234BC3A1AF}" type="CELLRANGE">
+                    <a:fld id="{C12D3AB7-CB7E-451F-AF33-C29DD195A786}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3535,7 +3554,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{BD2BD9D5-FAFD-4923-AC81-8233F5AF65E1}" type="PERCENTAGE">
+                    <a:fld id="{6E26CEC0-9DC8-4D13-BE7D-525226A5CC61}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3568,7 +3587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED835CEE-9BB3-4A27-B547-5826209068BD}" type="CELLRANGE">
+                    <a:fld id="{11F97178-8D59-4E9D-90DA-1A750A164303}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3577,7 +3596,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{B8968502-56BA-49F8-9F4E-38BF16AAD829}" type="PERCENTAGE">
+                    <a:fld id="{5E434219-B617-4D54-AC9D-6126F858BB99}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3942,7 +3961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74435343-AC85-43AC-B9E1-243E6696F717}" type="CELLRANGE">
+                    <a:fld id="{2EBA8149-3F41-4765-8327-34F4058F5424}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3951,7 +3970,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{001D7DB2-E0E8-46EB-8DF4-92F40E99FCEF}" type="PERCENTAGE">
+                    <a:fld id="{E2F0FAC6-0F3E-41F1-949F-19D2F3641863}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3984,7 +4003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09D2820D-A40E-4E14-871D-7CE18CD9E621}" type="CELLRANGE">
+                    <a:fld id="{72DC4A9F-8773-4BB0-A328-28ADF1186D6C}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3993,7 +4012,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{81814BE4-5701-4762-BDD5-734D30045414}" type="PERCENTAGE">
+                    <a:fld id="{47DEB5EF-B6AE-487F-A0B9-3BB78AD709A5}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -4026,7 +4045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{881AC11D-FF9A-49EE-AB29-25F8E8334F89}" type="CELLRANGE">
+                    <a:fld id="{C717C9BE-6A83-4B6B-AF14-C912C5119ABC}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4035,7 +4054,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{C8754553-48AA-4975-9B64-B5BE67CFBA6C}" type="PERCENTAGE">
+                    <a:fld id="{CE135722-8BDF-4E6B-8471-79DC92AFA8FA}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -7917,16 +7936,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>396128</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>198008</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>565184</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>367064</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7949,7 +7968,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8961008" y="0"/>
+          <a:off x="10294508" y="7620"/>
           <a:ext cx="2607456" cy="1889760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7962,15 +7981,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>102810</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>323790</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>517511</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>117650</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>128891</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>125270</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7993,7 +8012,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9886890" y="2034540"/>
+          <a:off x="10420290" y="2407920"/>
           <a:ext cx="3462701" cy="2456990"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12743,8 +12762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15257,8 +15276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1930402-D799-4BFF-9E29-635AB75B75C8}">
   <dimension ref="A2:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15493,7 +15512,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="str">
+      <c r="A12" s="55" t="str">
         <f t="shared" ref="A12:A13" si="1">+UPPER(A6)</f>
         <v>FEB</v>
       </c>
@@ -15505,7 +15524,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="55">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -15654,6 +15673,16 @@
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P29" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B35" s="67" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -15934,8 +15963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6A182A-4FB5-4415-8AA7-37C1E232FE20}">
   <dimension ref="A1:AF203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18486,7 +18515,6 @@
       <c r="E66"/>
     </row>
     <row r="67" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C67"/>
       <c r="D67"/>
       <c r="E67"/>
     </row>
@@ -18598,8 +18626,10 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C76"/>
+    <row r="76" spans="3:13" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="C76" s="67" t="s">
+        <v>163</v>
+      </c>
       <c r="D76"/>
       <c r="E76"/>
     </row>
@@ -21513,7 +21543,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21524,6 +21554,7 @@
     <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.3">
@@ -21534,6 +21565,9 @@
     <row r="2" spans="1:15" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="65"/>
       <c r="B2" s="66" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="66" t="s">
         <v>157</v>
       </c>
     </row>
@@ -21752,6 +21786,9 @@
       <c r="B11" s="66" t="s">
         <v>157</v>
       </c>
+      <c r="D11" s="66" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A12" s="63" t="s">
@@ -21763,29 +21800,29 @@
       <c r="C12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="F12" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="H12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="K12" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -21799,28 +21836,28 @@
         <v>2022</v>
       </c>
       <c r="D13" s="14">
+        <v>2</v>
+      </c>
+      <c r="E13" s="14">
         <v>731</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="F13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="17">
+      <c r="G13" s="17">
         <v>3313414.59</v>
       </c>
-      <c r="G13" s="17">
+      <c r="H13" s="17">
         <v>0</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="I13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>44816</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="K13" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -21834,28 +21871,28 @@
         <v>2022</v>
       </c>
       <c r="D14" s="6">
+        <v>2</v>
+      </c>
+      <c r="E14" s="6">
         <v>731</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="F14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="10">
+      <c r="G14" s="10">
         <v>0</v>
       </c>
-      <c r="G14" s="10">
+      <c r="H14" s="10">
         <v>200000</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>44816</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="K14" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -21869,28 +21906,28 @@
         <v>2022</v>
       </c>
       <c r="D15" s="6">
+        <v>2</v>
+      </c>
+      <c r="E15" s="6">
         <v>300</v>
       </c>
-      <c r="E15" s="12">
+      <c r="F15" s="12">
         <v>3004648676658</v>
       </c>
-      <c r="F15" s="10">
+      <c r="G15" s="10">
         <v>256200000</v>
       </c>
-      <c r="G15" s="10">
+      <c r="H15" s="10">
         <v>0</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="I15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>44816</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="K15" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -21904,28 +21941,28 @@
         <v>2022</v>
       </c>
       <c r="D16" s="6">
+        <v>2</v>
+      </c>
+      <c r="E16" s="6">
         <v>300</v>
       </c>
-      <c r="E16" s="12">
+      <c r="F16" s="12">
         <v>3004648676659</v>
       </c>
-      <c r="F16" s="10">
+      <c r="G16" s="10">
         <v>102124000</v>
       </c>
-      <c r="G16" s="10">
+      <c r="H16" s="10">
         <v>0</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>44816</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="K16" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -21939,26 +21976,26 @@
         <v>2022</v>
       </c>
       <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6">
         <v>300</v>
       </c>
-      <c r="E17" s="12">
+      <c r="F17" s="12">
         <v>3004648676660</v>
       </c>
-      <c r="F17" s="10">
+      <c r="G17" s="10">
         <v>4520000</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>44816</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="K17" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -21972,28 +22009,28 @@
         <v>2022</v>
       </c>
       <c r="D18" s="6">
+        <v>2</v>
+      </c>
+      <c r="E18" s="6">
         <v>731</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="F18" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="10">
+      <c r="G18" s="10">
         <v>5635000</v>
       </c>
-      <c r="G18" s="10">
+      <c r="H18" s="10">
         <v>0</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>44816</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="K18" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrega cambios de de cambios 3 y 4
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Fechas_Indicadores.xlsx
+++ b/app/dataextraction/Recibos/Fechas_Indicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266935E7-4832-4E41-A845-3CB0CC746813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A687E143-0384-42C8-A743-8170D84FBCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes " sheetId="1" r:id="rId1"/>
@@ -3503,7 +3503,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{37B6BF7C-A9E0-4BF8-9CDD-7059A03AA5CA}" type="CELLRANGE">
+                    <a:fld id="{98F66E5E-D82C-42CF-B215-D70FEE30CE80}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3512,7 +3512,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{15891FB5-7C87-46C1-A75C-D6327D607D15}" type="PERCENTAGE">
+                    <a:fld id="{8DD529B2-5921-4377-829C-40313BA502D2}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3545,7 +3545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C12D3AB7-CB7E-451F-AF33-C29DD195A786}" type="CELLRANGE">
+                    <a:fld id="{714C42AF-E231-4BD4-8F82-6E335D3D0B2A}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3554,7 +3554,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{6E26CEC0-9DC8-4D13-BE7D-525226A5CC61}" type="PERCENTAGE">
+                    <a:fld id="{75DFB7BD-4A35-4F51-97DB-06352C0E30A7}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3587,7 +3587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11F97178-8D59-4E9D-90DA-1A750A164303}" type="CELLRANGE">
+                    <a:fld id="{53768E3E-BE74-47CD-ADCF-A684B73B4535}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3596,7 +3596,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{5E434219-B617-4D54-AC9D-6126F858BB99}" type="PERCENTAGE">
+                    <a:fld id="{2E8D348E-45ED-465F-813C-9A3A4A5056A2}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -3961,7 +3961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EBA8149-3F41-4765-8327-34F4058F5424}" type="CELLRANGE">
+                    <a:fld id="{0A02E2FD-2C97-43C2-B902-DD5A9E7FFB23}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3970,7 +3970,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{E2F0FAC6-0F3E-41F1-949F-19D2F3641863}" type="PERCENTAGE">
+                    <a:fld id="{4D482A6C-E37A-4CF4-9D18-EFF951CBBCC4}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -4003,7 +4003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72DC4A9F-8773-4BB0-A328-28ADF1186D6C}" type="CELLRANGE">
+                    <a:fld id="{3E152E10-0562-4F7C-9EB8-C8576E4AA6A5}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4012,7 +4012,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{47DEB5EF-B6AE-487F-A0B9-3BB78AD709A5}" type="PERCENTAGE">
+                    <a:fld id="{87A196BF-4A61-4D94-9A1A-D41711D52AF0}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -4045,7 +4045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C717C9BE-6A83-4B6B-AF14-C912C5119ABC}" type="CELLRANGE">
+                    <a:fld id="{98496037-B724-4DF4-AB13-8D47F1340E9C}" type="CELLRANGE">
                       <a:rPr lang="es-AR"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4054,7 +4054,7 @@
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{CE135722-8BDF-4E6B-8471-79DC92AFA8FA}" type="PERCENTAGE">
+                    <a:fld id="{081BEF30-9F77-4259-B893-00BE124CF67A}" type="PERCENTAGE">
                       <a:rPr lang="es-AR" baseline="0"/>
                       <a:pPr/>
                       <a:t>[PERCENTAGE]</a:t>
@@ -12762,7 +12762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
@@ -15276,8 +15276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1930402-D799-4BFF-9E29-635AB75B75C8}">
   <dimension ref="A2:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15963,7 +15963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6A182A-4FB5-4415-8AA7-37C1E232FE20}">
   <dimension ref="A1:AF203"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>

</xml_diff>